<commit_message>
Added PTUC HTTT HD
</commit_message>
<xml_diff>
--- a/DH/PTUD HTTT HD/Topic/DanhSachTimHieuChuDe.xlsx
+++ b/DH/PTUD HTTT HD/Topic/DanhSachTimHieuChuDe.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Node.js</t>
   </si>
@@ -73,6 +73,10 @@
     <t xml:space="preserve">Võ Thanh Bình (1542211),
 Bùi Huy Bình (1542208)
 </t>
+  </si>
+  <si>
+    <t>1542250: Nguyễn Thanh Nhàn, 
+1542289: Nguyễn Thị Trí Tuệ</t>
   </si>
 </sst>
 </file>
@@ -451,7 +455,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D9" sqref="D9"/>
+      <selection pane="topRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -460,7 +464,7 @@
     <col min="2" max="2" width="31.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="97.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -498,7 +502,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -510,6 +514,9 @@
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added DH/PTUD HTTT HD/Topic/DanhSachTimHieuChuDe.xlsx
</commit_message>
<xml_diff>
--- a/DH/PTUD HTTT HD/Topic/DanhSachTimHieuChuDe.xlsx
+++ b/DH/PTUD HTTT HD/Topic/DanhSachTimHieuChuDe.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Node.js</t>
   </si>
@@ -77,13 +77,22 @@
   <si>
     <t>1542250: Nguyễn Thanh Nhàn, 
 1542289: Nguyễn Thị Trí Tuệ</t>
+  </si>
+  <si>
+    <t>Thời gian seminar</t>
+  </si>
+  <si>
+    <t>28/04/2017</t>
+  </si>
+  <si>
+    <t>05/05/2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +109,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -139,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -149,6 +165,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,11 +473,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E8" sqref="E8"/>
+      <selection pane="topRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -465,10 +487,11 @@
     <col min="3" max="3" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="97.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -484,8 +507,11 @@
       <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -501,8 +527,11 @@
       <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="F2" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -518,8 +547,11 @@
       <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="F3" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -532,8 +564,9 @@
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -546,6 +579,7 @@
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="F5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>